<commit_message>
Completed LDA code and added visualizations
</commit_message>
<xml_diff>
--- a/list_of_farmers_markets.xlsx
+++ b/list_of_farmers_markets.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8627e9ed649a0b00/Documents/GitHub/farmers-market/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adity\OneDrive\Documents\GitHub\farmers-market\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="8_{12C80E12-62C6-4FA6-926B-C152B3FD255E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{87422AA6-1F05-46B9-A10B-7F6395771B17}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="8_{12C80E12-62C6-4FA6-926B-C152B3FD255E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{74B77E92-2A7E-41E4-A01B-14CA33B340D2}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1073" windowWidth="28800" windowHeight="11422" xr2:uid="{E6EE6988-5896-4DD5-8103-E6EF094B9060}"/>
   </bookViews>
@@ -74,12 +74,6 @@
     <t>@DaneCoFM</t>
   </si>
   <si>
-    <t>Phildelphia, PA</t>
-  </si>
-  <si>
-    <t>Portland. OR</t>
-  </si>
-  <si>
     <t>New York, NY</t>
   </si>
   <si>
@@ -99,6 +93,12 @@
   </si>
   <si>
     <t>Madison, WI</t>
+  </si>
+  <si>
+    <t>Philadelphia, PA</t>
+  </si>
+  <si>
+    <t>Portland, OR</t>
   </si>
 </sst>
 </file>
@@ -464,7 +464,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -487,7 +487,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -498,7 +498,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
@@ -509,7 +509,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
@@ -520,7 +520,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
@@ -531,7 +531,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>7</v>
@@ -542,7 +542,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>8</v>
@@ -553,7 +553,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>9</v>
@@ -564,7 +564,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>10</v>
@@ -575,7 +575,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>11</v>
@@ -586,7 +586,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>12</v>

</xml_diff>